<commit_message>
Tiempos de algoritmos + Gráfico en excel
</commit_message>
<xml_diff>
--- a/EjecucionPruebas/Analisis_Algoritmos.xlsx
+++ b/EjecucionPruebas/Analisis_Algoritmos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Recursiva</t>
   </si>
@@ -46,6 +46,9 @@
   <si>
     <t>MathPow</t>
   </si>
+  <si>
+    <t>Tiempo en ms</t>
+  </si>
 </sst>
 </file>
 
@@ -60,15 +63,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -76,13 +85,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,198 +313,222 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$33</c:f>
+              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>499</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>999</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1499</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1999</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2499</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2999</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3499</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3999</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4499</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4999</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5499</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5999</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6499</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6999</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7499</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7999</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8499</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8999</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9499</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9999</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10499</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10999</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11499</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11999</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12499</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12999</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13499</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13999</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14499</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14999</c:v>
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$B$4:$B$33</c:f>
+              <c:f>'Datos + Gráfico'!$B$4:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>0.98199999999999998</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9990000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5569999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.03</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1950000000000003</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3639999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0259999999999998</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.3529999999999998</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.785</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.420999999999999</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.625</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>67.471999999999994</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>83.488</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>119.49299999999999</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>114.825</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>139.518</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>159.684</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>182.19200000000001</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>177.245</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>173.47900000000001</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>204.446</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>201.191</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>198.49100000000001</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>228.28899999999999</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>225.977</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>274.233</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>345.17899999999997</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>340.28</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>336.16699999999997</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>333.10500000000002</c:v>
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,198 +568,222 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$33</c:f>
+              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>499</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>999</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1499</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1999</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2499</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2999</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3499</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3999</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4499</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4999</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5499</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5999</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6499</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6999</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7499</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7999</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8499</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8999</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9499</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9999</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10499</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10999</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11499</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11999</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12499</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12999</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13499</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13999</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14499</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14999</c:v>
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$C$4:$C$33</c:f>
+              <c:f>'Datos + Gráfico'!$C$4:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>1.101</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1280000000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2130000000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1640000000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1509999999999998</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.763999999999999</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.803000000000001</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.124000000000001</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25.091000000000001</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.41</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.362000000000002</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>70.248000000000005</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76.191000000000003</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>111.682</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>108.61799999999999</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>106.571</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>117.628</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>163.57300000000001</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>160.24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>157.923</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>238.911</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>234.24100000000001</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>316.02100000000002</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>359.61599999999999</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>399.73899999999998</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>391.39800000000002</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>443.47500000000002</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>488.68799999999999</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>479.74299999999999</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>510.51499999999999</c:v>
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -666,198 +823,222 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$33</c:f>
+              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>499</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>999</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1499</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1999</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2499</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2999</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3499</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3999</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4499</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4999</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5499</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5999</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6499</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6999</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7499</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7999</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8499</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8999</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9499</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9999</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10499</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10999</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11499</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11999</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12499</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12999</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13499</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13999</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14499</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14999</c:v>
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$D$4:$D$33</c:f>
+              <c:f>'Datos + Gráfico'!$D$4:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>0.57099999999999995</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6559999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.512</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.556</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0049999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5670000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.3490000000000002</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.258</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.146000000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.930999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.041</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.113</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.384</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25.946999999999999</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40.697000000000003</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>39.76</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>39.075000000000003</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>70.944000000000003</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>75.141000000000005</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>110.28400000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>151.983</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>147.095</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>142.803</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>139.346</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>136.11199999999999</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>133.41800000000001</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>130.93899999999999</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>128.673</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>185.321</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>241.68299999999999</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,7 +1059,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Horner</c:v>
+                  <c:v>ProgDinamica</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -897,198 +1078,222 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$33</c:f>
+              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>499</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>999</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1499</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1999</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2499</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2999</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3499</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3999</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4499</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4999</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5499</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5999</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6499</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6999</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7499</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7999</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8499</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8999</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9499</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9999</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10499</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10999</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11499</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11999</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12499</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12999</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13499</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13999</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14499</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14999</c:v>
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$E$4:$E$33</c:f>
+              <c:f>'Datos + Gráfico'!$E$4:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>1.9E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.331</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.423</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.718</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.085</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4590000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.871</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.342000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.547999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.828000000000003</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49.963999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47.088999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>52.494999999999997</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50.11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>63.401000000000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>83.262</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>80.072000000000003</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>111.405</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>107.426</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>128.58500000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>149.529</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>145.15199999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>168.91</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>164.363</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>159.93899999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>156.09</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>193.84299999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>247.41300000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>305.23700000000002</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1109,7 +1314,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ProgDinamica</c:v>
+                  <c:v>MathPow</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1128,198 +1333,222 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$33</c:f>
+              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>499</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>999</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1499</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1999</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2499</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2999</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3499</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3999</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4499</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4999</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5499</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5999</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6499</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6999</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7499</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7999</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8499</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8999</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9499</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9999</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10499</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10999</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11499</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11999</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12499</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12999</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13499</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13999</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14499</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14999</c:v>
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$F$4:$F$33</c:f>
+              <c:f>'Datos + Gráfico'!$F$4:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>2.3E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.177</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1759999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4870000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.081</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2109999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4420000000000002</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7650000000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1960000000000002</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9729999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.7309999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.2640000000000002</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.8209999999999997</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.327</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32.524999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32.85</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>59.581000000000003</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>91.819000000000003</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>108.53700000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>136.17099999999999</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>131.47499999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>127.36199999999999</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>141.547</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>185.97399999999999</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>180.50399999999999</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>175.64400000000001</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>171.292</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>220.81899999999999</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>215.60400000000001</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>219.911</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1340,7 +1569,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MathPow</c:v>
+                  <c:v>Horner</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1359,198 +1588,222 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$33</c:f>
+              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>499</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>999</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1499</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1999</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2499</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2999</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3499</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3999</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4499</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4999</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5499</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5999</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6499</c:v>
+                  <c:v>2800</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6999</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7499</c:v>
+                  <c:v>3200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7999</c:v>
+                  <c:v>3400</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8499</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8999</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9499</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9999</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10499</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10999</c:v>
+                  <c:v>4600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11499</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11999</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12499</c:v>
+                  <c:v>5200</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12999</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13499</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13999</c:v>
+                  <c:v>5800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14499</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14999</c:v>
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$G$4:$G$33</c:f>
+              <c:f>'Datos + Gráfico'!$G$4:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>7.9000000000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3149999999999999</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.399</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.472</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6560000000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.79</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.153</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.794</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.7069999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.1379999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.8559999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.5739999999999998</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.37</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.786000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51.567</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>69.53</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>66.965000000000003</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>72.869</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>70.593000000000004</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>68.587999999999994</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>67.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>100.81100000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>145.761</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>152.565</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>148.68100000000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>145.21899999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>142.02699999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>178.55</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>174.767</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>235.43100000000001</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2318,16 +2571,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>481011</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>100010</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2612,762 +2865,965 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G33"/>
+  <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="2" max="7" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>400</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>600</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>800</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1200</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1400</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1600</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1800</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2200</v>
+      </c>
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2400</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2600</v>
+      </c>
+      <c r="B15" s="8">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2800</v>
+      </c>
+      <c r="B16" s="8">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>11</v>
+      </c>
+      <c r="D16" s="4">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>3000</v>
+      </c>
+      <c r="B17" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>499</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.101</v>
-      </c>
-      <c r="D4">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="E4">
-        <v>1.9E-2</v>
-      </c>
-      <c r="F4">
-        <v>2.3E-2</v>
-      </c>
-      <c r="G4">
-        <v>7.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>A4+500</f>
-        <v>999</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1.9990000000000001</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.1280000000000001</v>
-      </c>
-      <c r="D5">
-        <v>1.6559999999999999</v>
-      </c>
-      <c r="E5">
-        <v>1.331</v>
-      </c>
-      <c r="F5">
-        <v>1.177</v>
-      </c>
-      <c r="G5">
-        <v>1.3149999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" ref="A6:A33" si="0">A5+500</f>
-        <v>1499</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2.5569999999999999</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.2130000000000001</v>
-      </c>
-      <c r="D6">
-        <v>1.512</v>
-      </c>
-      <c r="E6">
-        <v>1.423</v>
-      </c>
-      <c r="F6">
-        <v>1.1759999999999999</v>
-      </c>
-      <c r="G6">
-        <v>1.399</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>1999</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3.03</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3.1640000000000001</v>
-      </c>
-      <c r="D7">
-        <v>1.556</v>
-      </c>
-      <c r="E7">
-        <v>1.718</v>
-      </c>
-      <c r="F7">
-        <v>1.4870000000000001</v>
-      </c>
-      <c r="G7">
-        <v>2.472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>2499</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7.1950000000000003</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7.1509999999999998</v>
-      </c>
-      <c r="D8">
-        <v>2.0049999999999999</v>
-      </c>
-      <c r="E8">
-        <v>2.75</v>
-      </c>
-      <c r="F8">
-        <v>2.081</v>
-      </c>
-      <c r="G8">
-        <v>2.6560000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>2999</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7.3639999999999999</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10.763999999999999</v>
-      </c>
-      <c r="D9">
-        <v>7.5670000000000002</v>
-      </c>
-      <c r="E9">
-        <v>3.085</v>
-      </c>
-      <c r="F9">
-        <v>2.2109999999999999</v>
-      </c>
-      <c r="G9">
-        <v>2.79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>3499</v>
-      </c>
-      <c r="B10" s="1">
-        <v>8.0259999999999998</v>
-      </c>
-      <c r="C10" s="1">
-        <v>13.803000000000001</v>
-      </c>
-      <c r="D10">
-        <v>7.3490000000000002</v>
-      </c>
-      <c r="E10">
-        <v>3.4590000000000001</v>
-      </c>
-      <c r="F10">
-        <v>2.4420000000000002</v>
-      </c>
-      <c r="G10">
-        <v>3.153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>3999</v>
-      </c>
-      <c r="B11" s="1">
-        <v>9.3529999999999998</v>
-      </c>
-      <c r="C11" s="1">
-        <v>14.124000000000001</v>
-      </c>
-      <c r="D11">
-        <v>7.258</v>
-      </c>
-      <c r="E11">
-        <v>15.871</v>
-      </c>
-      <c r="F11">
-        <v>2.7650000000000001</v>
-      </c>
-      <c r="G11">
-        <v>3.794</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>4499</v>
-      </c>
-      <c r="B12" s="1">
-        <v>21.785</v>
-      </c>
-      <c r="C12" s="1">
-        <v>25.091000000000001</v>
-      </c>
-      <c r="D12">
-        <v>13.146000000000001</v>
-      </c>
-      <c r="E12">
-        <v>15.342000000000001</v>
-      </c>
-      <c r="F12">
-        <v>3.1960000000000002</v>
-      </c>
-      <c r="G12">
-        <v>4.7069999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>4999</v>
-      </c>
-      <c r="B13" s="1">
-        <v>31.420999999999999</v>
-      </c>
-      <c r="C13" s="1">
-        <v>31.41</v>
-      </c>
-      <c r="D13">
-        <v>12.930999999999999</v>
-      </c>
-      <c r="E13">
-        <v>29.547999999999998</v>
-      </c>
-      <c r="F13">
-        <v>3.9729999999999999</v>
-      </c>
-      <c r="G13">
-        <v>5.1379999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>5499</v>
-      </c>
-      <c r="B14" s="1">
-        <v>31.625</v>
-      </c>
-      <c r="C14" s="1">
-        <v>50.362000000000002</v>
-      </c>
-      <c r="D14">
-        <v>13.041</v>
-      </c>
-      <c r="E14">
-        <v>32.828000000000003</v>
-      </c>
-      <c r="F14">
-        <v>4.7309999999999999</v>
-      </c>
-      <c r="G14">
-        <v>5.8559999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>5999</v>
-      </c>
-      <c r="B15" s="1">
-        <v>67.471999999999994</v>
-      </c>
-      <c r="C15" s="1">
-        <v>70.248000000000005</v>
-      </c>
-      <c r="D15">
-        <v>13.113</v>
-      </c>
-      <c r="E15">
-        <v>49.963999999999999</v>
-      </c>
-      <c r="F15">
-        <v>7.2640000000000002</v>
-      </c>
-      <c r="G15">
-        <v>6.5739999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>6499</v>
-      </c>
-      <c r="B16" s="1">
-        <v>83.488</v>
-      </c>
-      <c r="C16" s="1">
-        <v>76.191000000000003</v>
-      </c>
-      <c r="D16">
-        <v>13.384</v>
-      </c>
-      <c r="E16">
-        <v>47.088999999999999</v>
-      </c>
-      <c r="F16">
-        <v>7.8209999999999997</v>
-      </c>
-      <c r="G16">
-        <v>7.37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>6999</v>
-      </c>
-      <c r="B17" s="1">
-        <v>119.49299999999999</v>
-      </c>
-      <c r="C17" s="1">
-        <v>111.682</v>
-      </c>
-      <c r="D17">
-        <v>25.946999999999999</v>
-      </c>
-      <c r="E17">
-        <v>52.494999999999997</v>
-      </c>
-      <c r="F17">
-        <v>8.327</v>
-      </c>
-      <c r="G17">
-        <v>32.786000000000001</v>
+      <c r="C17" s="6">
+        <v>14</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>7499</v>
-      </c>
-      <c r="B18" s="1">
-        <v>114.825</v>
-      </c>
-      <c r="C18" s="1">
-        <v>108.61799999999999</v>
-      </c>
-      <c r="D18">
-        <v>40.697000000000003</v>
-      </c>
-      <c r="E18">
-        <v>50.11</v>
-      </c>
-      <c r="F18">
-        <v>32.524999999999999</v>
-      </c>
-      <c r="G18">
-        <v>51.567</v>
+      <c r="A18" s="4">
+        <v>3200</v>
+      </c>
+      <c r="B18" s="8">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>7999</v>
-      </c>
-      <c r="B19" s="1">
-        <v>139.518</v>
-      </c>
-      <c r="C19" s="1">
-        <v>106.571</v>
-      </c>
-      <c r="D19">
-        <v>39.76</v>
-      </c>
-      <c r="E19">
-        <v>63.401000000000003</v>
-      </c>
-      <c r="F19">
-        <v>32.85</v>
-      </c>
-      <c r="G19">
-        <v>69.53</v>
+      <c r="A19" s="4">
+        <v>3400</v>
+      </c>
+      <c r="B19" s="8">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>8499</v>
-      </c>
-      <c r="B20" s="1">
-        <v>159.684</v>
-      </c>
-      <c r="C20" s="1">
-        <v>117.628</v>
-      </c>
-      <c r="D20">
-        <v>39.075000000000003</v>
-      </c>
-      <c r="E20">
-        <v>83.262</v>
-      </c>
-      <c r="F20">
-        <v>59.581000000000003</v>
-      </c>
-      <c r="G20">
-        <v>66.965000000000003</v>
+      <c r="A20" s="4">
+        <v>3600</v>
+      </c>
+      <c r="B20" s="8">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6">
+        <v>19</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>2</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>8999</v>
-      </c>
-      <c r="B21" s="1">
-        <v>182.19200000000001</v>
-      </c>
-      <c r="C21" s="1">
-        <v>163.57300000000001</v>
-      </c>
-      <c r="D21">
-        <v>70.944000000000003</v>
-      </c>
-      <c r="E21">
-        <v>80.072000000000003</v>
-      </c>
-      <c r="F21">
-        <v>91.819000000000003</v>
-      </c>
-      <c r="G21">
-        <v>72.869</v>
+      <c r="A21" s="4">
+        <v>3800</v>
+      </c>
+      <c r="B21" s="8">
+        <v>9</v>
+      </c>
+      <c r="C21" s="6">
+        <v>20</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>2</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>9499</v>
-      </c>
-      <c r="B22" s="1">
-        <v>177.245</v>
-      </c>
-      <c r="C22" s="1">
-        <v>160.24</v>
-      </c>
-      <c r="D22">
-        <v>75.141000000000005</v>
-      </c>
-      <c r="E22">
-        <v>111.405</v>
-      </c>
-      <c r="F22">
-        <v>108.53700000000001</v>
-      </c>
-      <c r="G22">
-        <v>70.593000000000004</v>
+      <c r="A22" s="4">
+        <v>4000</v>
+      </c>
+      <c r="B22" s="8">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6">
+        <v>23</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>9999</v>
-      </c>
-      <c r="B23" s="1">
-        <v>173.47900000000001</v>
-      </c>
-      <c r="C23" s="1">
-        <v>157.923</v>
-      </c>
-      <c r="D23">
-        <v>110.28400000000001</v>
-      </c>
-      <c r="E23">
-        <v>107.426</v>
-      </c>
-      <c r="F23">
-        <v>136.17099999999999</v>
-      </c>
-      <c r="G23">
-        <v>68.587999999999994</v>
+      <c r="A23" s="4">
+        <v>4200</v>
+      </c>
+      <c r="B23" s="8">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6">
+        <v>25</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>10499</v>
-      </c>
-      <c r="B24">
-        <v>204.446</v>
-      </c>
-      <c r="C24">
-        <v>238.911</v>
-      </c>
-      <c r="D24">
-        <v>151.983</v>
-      </c>
-      <c r="E24">
-        <v>128.58500000000001</v>
-      </c>
-      <c r="F24">
-        <v>131.47499999999999</v>
-      </c>
-      <c r="G24">
-        <v>67.2</v>
+      <c r="A24" s="4">
+        <v>4400</v>
+      </c>
+      <c r="B24" s="9">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4">
+        <v>27</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>10999</v>
-      </c>
-      <c r="B25">
-        <v>201.191</v>
-      </c>
-      <c r="C25">
-        <v>234.24100000000001</v>
-      </c>
-      <c r="D25">
-        <v>147.095</v>
-      </c>
-      <c r="E25">
-        <v>149.529</v>
-      </c>
-      <c r="F25">
-        <v>127.36199999999999</v>
-      </c>
-      <c r="G25">
-        <v>100.81100000000001</v>
+      <c r="A25" s="4">
+        <v>4600</v>
+      </c>
+      <c r="B25" s="9">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4">
+        <v>31</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>11499</v>
-      </c>
-      <c r="B26">
-        <v>198.49100000000001</v>
-      </c>
-      <c r="C26">
-        <v>316.02100000000002</v>
-      </c>
-      <c r="D26">
-        <v>142.803</v>
-      </c>
-      <c r="E26">
-        <v>145.15199999999999</v>
-      </c>
-      <c r="F26">
-        <v>141.547</v>
-      </c>
-      <c r="G26">
-        <v>145.761</v>
+      <c r="A26" s="4">
+        <v>4800</v>
+      </c>
+      <c r="B26" s="9">
+        <v>14</v>
+      </c>
+      <c r="C26" s="4">
+        <v>33</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>11999</v>
-      </c>
-      <c r="B27">
-        <v>228.28899999999999</v>
-      </c>
-      <c r="C27">
-        <v>359.61599999999999</v>
-      </c>
-      <c r="D27">
-        <v>139.346</v>
-      </c>
-      <c r="E27">
-        <v>168.91</v>
-      </c>
-      <c r="F27">
-        <v>185.97399999999999</v>
-      </c>
-      <c r="G27">
-        <v>152.565</v>
+      <c r="A27" s="4">
+        <v>5000</v>
+      </c>
+      <c r="B27" s="9">
+        <v>14</v>
+      </c>
+      <c r="C27" s="4">
+        <v>37</v>
+      </c>
+      <c r="D27" s="4">
+        <v>3</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>12499</v>
-      </c>
-      <c r="B28">
-        <v>225.977</v>
-      </c>
-      <c r="C28">
-        <v>399.73899999999998</v>
-      </c>
-      <c r="D28">
-        <v>136.11199999999999</v>
-      </c>
-      <c r="E28">
-        <v>164.363</v>
-      </c>
-      <c r="F28">
-        <v>180.50399999999999</v>
-      </c>
-      <c r="G28">
-        <v>148.68100000000001</v>
+      <c r="A28" s="4">
+        <v>5200</v>
+      </c>
+      <c r="B28" s="9">
+        <v>16</v>
+      </c>
+      <c r="C28" s="4">
+        <v>39</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>12999</v>
-      </c>
-      <c r="B29">
-        <v>274.233</v>
-      </c>
-      <c r="C29">
-        <v>391.39800000000002</v>
-      </c>
-      <c r="D29">
-        <v>133.41800000000001</v>
-      </c>
-      <c r="E29">
-        <v>159.93899999999999</v>
-      </c>
-      <c r="F29">
-        <v>175.64400000000001</v>
-      </c>
-      <c r="G29">
-        <v>145.21899999999999</v>
+      <c r="A29" s="4">
+        <v>5400</v>
+      </c>
+      <c r="B29" s="9">
+        <v>17</v>
+      </c>
+      <c r="C29" s="4">
+        <v>42</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>13499</v>
-      </c>
-      <c r="B30">
-        <v>345.17899999999997</v>
-      </c>
-      <c r="C30">
-        <v>443.47500000000002</v>
-      </c>
-      <c r="D30">
-        <v>130.93899999999999</v>
-      </c>
-      <c r="E30">
-        <v>156.09</v>
-      </c>
-      <c r="F30">
-        <v>171.292</v>
-      </c>
-      <c r="G30">
-        <v>142.02699999999999</v>
+      <c r="A30" s="4">
+        <v>5600</v>
+      </c>
+      <c r="B30" s="9">
+        <v>18</v>
+      </c>
+      <c r="C30" s="4">
+        <v>44</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>13999</v>
-      </c>
-      <c r="B31">
-        <v>340.28</v>
-      </c>
-      <c r="C31">
-        <v>488.68799999999999</v>
-      </c>
-      <c r="D31">
-        <v>128.673</v>
-      </c>
-      <c r="E31">
-        <v>193.84299999999999</v>
-      </c>
-      <c r="F31">
-        <v>220.81899999999999</v>
-      </c>
-      <c r="G31">
-        <v>178.55</v>
+      <c r="A31" s="4">
+        <v>5800</v>
+      </c>
+      <c r="B31" s="9">
+        <v>20</v>
+      </c>
+      <c r="C31" s="4">
+        <v>49</v>
+      </c>
+      <c r="D31" s="4">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>2</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>14499</v>
-      </c>
-      <c r="B32">
-        <v>336.16699999999997</v>
-      </c>
-      <c r="C32">
-        <v>479.74299999999999</v>
-      </c>
-      <c r="D32">
-        <v>185.321</v>
-      </c>
-      <c r="E32">
-        <v>247.41300000000001</v>
-      </c>
-      <c r="F32">
-        <v>215.60400000000001</v>
-      </c>
-      <c r="G32">
-        <v>174.767</v>
+      <c r="A32" s="4">
+        <v>6000</v>
+      </c>
+      <c r="B32" s="9">
+        <v>22</v>
+      </c>
+      <c r="C32" s="4">
+        <v>52</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>3</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>14999</v>
-      </c>
-      <c r="B33">
-        <v>333.10500000000002</v>
-      </c>
-      <c r="C33">
-        <v>510.51499999999999</v>
-      </c>
-      <c r="D33">
-        <v>241.68299999999999</v>
-      </c>
-      <c r="E33">
-        <v>305.23700000000002</v>
-      </c>
-      <c r="F33">
-        <v>219.911</v>
-      </c>
-      <c r="G33">
-        <v>235.43100000000001</v>
-      </c>
+      <c r="A33" s="4">
+        <v>6200</v>
+      </c>
+      <c r="B33" s="9">
+        <v>23</v>
+      </c>
+      <c r="C33" s="4">
+        <v>55</v>
+      </c>
+      <c r="D33" s="4">
+        <v>3</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>6400</v>
+      </c>
+      <c r="B34" s="9">
+        <v>25</v>
+      </c>
+      <c r="C34" s="4">
+        <v>59</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>6600</v>
+      </c>
+      <c r="B35" s="9">
+        <v>26</v>
+      </c>
+      <c r="C35" s="4">
+        <v>62</v>
+      </c>
+      <c r="D35" s="4">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>6800</v>
+      </c>
+      <c r="B36" s="9">
+        <v>27</v>
+      </c>
+      <c r="C36" s="4">
+        <v>67</v>
+      </c>
+      <c r="D36" s="4">
+        <v>3</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>3</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>7000</v>
+      </c>
+      <c r="B37" s="10">
+        <v>29</v>
+      </c>
+      <c r="C37" s="5">
+        <v>71</v>
+      </c>
+      <c r="D37" s="5">
+        <v>3</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>3</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>